<commit_message>
add and changed files via upload
</commit_message>
<xml_diff>
--- a/minimum_wage.xlsx
+++ b/minimum_wage.xlsx
@@ -584,26 +584,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -617,6 +602,21 @@
     </xf>
     <xf numFmtId="2" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -932,1321 +932,1491 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BC0F8E6-24EC-429D-A11A-EA62F0FC64F7}">
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="8.7265625" style="10"/>
+    <col min="1" max="16384" width="8.7265625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9">
+      <c r="B1" s="13">
         <v>2010</v>
       </c>
-      <c r="C1" s="9">
+      <c r="C1" s="13">
         <v>2011</v>
       </c>
-      <c r="D1" s="9">
+      <c r="D1" s="13">
         <v>2012</v>
       </c>
-      <c r="E1" s="9">
+      <c r="E1" s="13">
         <v>2013</v>
       </c>
-      <c r="F1" s="9">
+      <c r="F1" s="13">
         <v>2014</v>
       </c>
-      <c r="G1" s="9">
+      <c r="G1" s="13">
         <v>2015</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="11" t="s">
+      <c r="H1" s="13">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-    </row>
-    <row r="3" spans="1:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="14" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="15">
-        <v>7.25</v>
-      </c>
-      <c r="C3" s="15">
-        <v>7.25</v>
-      </c>
-      <c r="D3" s="15">
-        <v>7.25</v>
-      </c>
-      <c r="E3" s="15">
-        <v>7.25</v>
-      </c>
-      <c r="F3" s="15">
-        <v>7.25</v>
-      </c>
-      <c r="G3" s="15">
-        <v>7.25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="10">
+        <v>7.25</v>
+      </c>
+      <c r="C3" s="10">
+        <v>7.25</v>
+      </c>
+      <c r="D3" s="10">
+        <v>7.25</v>
+      </c>
+      <c r="E3" s="10">
+        <v>7.25</v>
+      </c>
+      <c r="F3" s="10">
+        <v>7.25</v>
+      </c>
+      <c r="G3" s="10">
+        <v>7.25</v>
+      </c>
+      <c r="H3" s="10">
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="C4" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="D4" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="E4" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="F4" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="G4" s="16">
-        <v>7.25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="C4" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="D4" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="E4" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="F4" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="G4" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="H4" s="11">
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="11">
         <v>7.75</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="11">
         <v>7.75</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="11">
         <v>7.75</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E5" s="11">
         <v>7.75</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="11">
         <v>7.75</v>
       </c>
-      <c r="G5" s="16">
+      <c r="G5" s="11">
         <v>8.75</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H5" s="11">
+        <v>9.75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="C6" s="16">
+      <c r="B6" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="C6" s="11">
         <v>7.35</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="11">
         <v>7.65</v>
       </c>
-      <c r="E6" s="16">
+      <c r="E6" s="11">
         <v>7.8</v>
       </c>
-      <c r="F6" s="16">
+      <c r="F6" s="11">
         <v>7.9</v>
       </c>
-      <c r="G6" s="16">
+      <c r="G6" s="11">
         <v>8.0500000000000007</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H6" s="11">
+        <v>8.0500000000000007</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="C7" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="D7" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="E7" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="F7" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="G7" s="16">
+      <c r="B7" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="C7" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="D7" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="E7" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="F7" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="G7" s="11">
         <v>7.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H7" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="16">
+      <c r="B8" s="11">
         <v>8</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="11">
         <v>8</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="11">
         <v>8</v>
       </c>
-      <c r="E8" s="16">
+      <c r="E8" s="11">
         <v>8</v>
       </c>
-      <c r="F8" s="16">
+      <c r="F8" s="11">
         <v>9</v>
       </c>
-      <c r="G8" s="16">
+      <c r="G8" s="11">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H8" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9" s="11">
         <v>7.24</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="11">
         <v>7.36</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="11">
         <v>7.64</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="11">
         <v>7.78</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="11">
         <v>8</v>
       </c>
-      <c r="G9" s="16">
+      <c r="G9" s="11">
         <v>8.23</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H9" s="11">
+        <v>8.31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="16">
+      <c r="B10" s="11">
         <v>8.25</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="11">
         <v>8.25</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="11">
         <v>8.25</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="11">
         <v>8.25</v>
       </c>
-      <c r="F10" s="16">
+      <c r="F10" s="11">
         <v>8.6999999999999993</v>
       </c>
-      <c r="G10" s="16">
+      <c r="G10" s="11">
         <v>9.15</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H10" s="11">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="C11" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="D11" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="E11" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="F11" s="16">
+      <c r="B11" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="C11" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="D11" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="E11" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="F11" s="11">
         <v>7.75</v>
       </c>
-      <c r="G11" s="16">
+      <c r="G11" s="11">
         <v>8.25</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H11" s="11">
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="C12" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="D12" s="16">
+      <c r="B12" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="C12" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="D12" s="11">
         <v>7.67</v>
       </c>
-      <c r="E12" s="16">
+      <c r="E12" s="11">
         <v>7.79</v>
       </c>
-      <c r="F12" s="16">
+      <c r="F12" s="11">
         <v>7.93</v>
       </c>
-      <c r="G12" s="16">
+      <c r="G12" s="11">
         <v>8.0500000000000007</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H12" s="11">
+        <v>8.0500000000000007</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="C13" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="D13" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="E13" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="F13" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="G13" s="16">
-        <v>7.25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="C13" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="D13" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="E13" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="F13" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="G13" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="H13" s="11">
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="C14" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="D14" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="E14" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="F14" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="G14" s="16">
+      <c r="B14" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="C14" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="D14" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="E14" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="F14" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="G14" s="11">
         <v>7.75</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H14" s="11">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="C15" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="D15" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="E15" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="F15" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="G15" s="16">
-        <v>7.25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B15" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="C15" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="D15" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="E15" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="F15" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="G15" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="H15" s="11">
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="16">
+      <c r="B16" s="11">
         <v>8</v>
       </c>
-      <c r="C16" s="16">
+      <c r="C16" s="11">
         <v>8.25</v>
       </c>
-      <c r="D16" s="16">
+      <c r="D16" s="11">
         <v>8.25</v>
       </c>
-      <c r="E16" s="16">
+      <c r="E16" s="11">
         <v>8.25</v>
       </c>
-      <c r="F16" s="16">
+      <c r="F16" s="11">
         <v>8.25</v>
       </c>
-      <c r="G16" s="16">
+      <c r="G16" s="11">
         <v>8.25</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H16" s="11">
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="C17" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="D17" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="E17" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="F17" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="G17" s="16">
-        <v>7.25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B17" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="C17" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="D17" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="E17" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="F17" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="G17" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="H17" s="11">
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="C18" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="D18" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="E18" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="F18" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="G18" s="16">
-        <v>7.25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B18" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="C18" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="D18" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="E18" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="F18" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="G18" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="H18" s="11">
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="C19" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="D19" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="E19" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="F19" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="G19" s="16">
-        <v>7.25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B19" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="C19" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="D19" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="E19" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="F19" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="G19" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="H19" s="11">
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="C20" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="D20" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="E20" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="F20" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="G20" s="16">
-        <v>7.25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B20" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="C20" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="D20" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="E20" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="F20" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="G20" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="H20" s="11">
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="C21" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="D21" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="E21" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="F21" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="G21" s="16">
-        <v>7.25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B21" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="C21" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="D21" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="E21" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="F21" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="G21" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="H21" s="11">
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="16">
+      <c r="B22" s="11">
         <v>7.5</v>
       </c>
-      <c r="C22" s="16">
+      <c r="C22" s="11">
         <v>7.5</v>
       </c>
-      <c r="D22" s="16">
+      <c r="D22" s="11">
         <v>7.5</v>
       </c>
-      <c r="E22" s="16">
+      <c r="E22" s="11">
         <v>7.5</v>
       </c>
-      <c r="F22" s="16">
+      <c r="F22" s="11">
         <v>7.5</v>
       </c>
-      <c r="G22" s="16">
+      <c r="G22" s="11">
         <v>7.5</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H22" s="11">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="C23" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="D23" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="E23" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="F23" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="G23" s="16">
+      <c r="B23" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="C23" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="D23" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="E23" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="F23" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="G23" s="11">
         <v>8.25</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H23" s="11">
+        <v>8.75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="16">
+      <c r="B24" s="11">
         <v>8</v>
       </c>
-      <c r="C24" s="16">
+      <c r="C24" s="11">
         <v>8</v>
       </c>
-      <c r="D24" s="16">
+      <c r="D24" s="11">
         <v>8</v>
       </c>
-      <c r="E24" s="16">
+      <c r="E24" s="11">
         <v>8</v>
       </c>
-      <c r="F24" s="16">
+      <c r="F24" s="11">
         <v>8</v>
       </c>
-      <c r="G24" s="16">
+      <c r="G24" s="11">
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H24" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="16">
+      <c r="B25" s="11">
         <v>7.4</v>
       </c>
-      <c r="C25" s="16">
+      <c r="C25" s="11">
         <v>7.4</v>
       </c>
-      <c r="D25" s="16">
+      <c r="D25" s="11">
         <v>7.4</v>
       </c>
-      <c r="E25" s="16">
+      <c r="E25" s="11">
         <v>7.4</v>
       </c>
-      <c r="F25" s="16">
+      <c r="F25" s="11">
         <v>8.15</v>
       </c>
-      <c r="G25" s="16">
+      <c r="G25" s="11">
         <v>8.15</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H25" s="11">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="C26" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="D26" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="E26" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="F26" s="16">
+      <c r="B26" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="C26" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="D26" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="E26" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="F26" s="11">
         <v>8</v>
       </c>
-      <c r="G26" s="16">
+      <c r="G26" s="11">
         <v>9</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H26" s="11">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="C27" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="D27" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="E27" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="F27" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="G27" s="16">
-        <v>7.25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B27" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="C27" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="D27" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="E27" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="F27" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="G27" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="H27" s="11">
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B28" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="C28" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="D28" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="E28" s="16">
+      <c r="B28" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="C28" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="D28" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="E28" s="11">
         <v>7.35</v>
       </c>
-      <c r="F28" s="16">
+      <c r="F28" s="11">
         <v>7.5</v>
       </c>
-      <c r="G28" s="16">
+      <c r="G28" s="11">
         <v>7.65</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H28" s="11">
+        <v>7.65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B29" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="C29" s="16">
+      <c r="B29" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="C29" s="11">
         <v>7.35</v>
       </c>
-      <c r="D29" s="16">
+      <c r="D29" s="11">
         <v>7.65</v>
       </c>
-      <c r="E29" s="16">
+      <c r="E29" s="11">
         <v>7.8</v>
       </c>
-      <c r="F29" s="16">
+      <c r="F29" s="11">
         <v>7.9</v>
       </c>
-      <c r="G29" s="16">
+      <c r="G29" s="11">
         <v>8.0500000000000007</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H29" s="11">
+        <v>8.0500000000000007</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="C30" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="D30" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="E30" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="F30" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="G30" s="16">
+      <c r="B30" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="C30" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="D30" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="E30" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="F30" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="G30" s="11">
         <v>8</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H30" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B31" s="16">
+      <c r="B31" s="11">
         <v>7.55</v>
       </c>
-      <c r="C31" s="16">
+      <c r="C31" s="11">
         <v>8.25</v>
       </c>
-      <c r="D31" s="16">
+      <c r="D31" s="11">
         <v>8.25</v>
       </c>
-      <c r="E31" s="16">
+      <c r="E31" s="11">
         <v>8.25</v>
       </c>
-      <c r="F31" s="16">
+      <c r="F31" s="11">
         <v>8.25</v>
       </c>
-      <c r="G31" s="16">
+      <c r="G31" s="11">
         <v>8.25</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H31" s="11">
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B32" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="C32" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="D32" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="E32" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="F32" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="G32" s="16">
-        <v>7.25</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B32" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="C32" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="D32" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="E32" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="F32" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="G32" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="H32" s="11">
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B33" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="C33" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="D33" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="E33" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="F33" s="16">
+      <c r="B33" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="C33" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="D33" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="E33" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="F33" s="11">
         <v>8.25</v>
       </c>
-      <c r="G33" s="16">
+      <c r="G33" s="11">
         <v>8.3800000000000008</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H33" s="11">
+        <v>8.3800000000000008</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B34" s="16">
+      <c r="B34" s="11">
         <v>7.5</v>
       </c>
-      <c r="C34" s="16">
+      <c r="C34" s="11">
         <v>7.5</v>
       </c>
-      <c r="D34" s="16">
+      <c r="D34" s="11">
         <v>7.5</v>
       </c>
-      <c r="E34" s="16">
+      <c r="E34" s="11">
         <v>7.5</v>
       </c>
-      <c r="F34" s="16">
+      <c r="F34" s="11">
         <v>7.5</v>
       </c>
-      <c r="G34" s="16">
+      <c r="G34" s="11">
         <v>7.5</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H34" s="11">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B35" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="C35" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="D35" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="E35" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="F35" s="16">
+      <c r="B35" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="C35" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="D35" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="E35" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="F35" s="11">
         <v>8</v>
       </c>
-      <c r="G35" s="16">
+      <c r="G35" s="11">
         <v>8.75</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H35" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B36" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="C36" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="D36" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="E36" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="F36" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="G36" s="16">
-        <v>7.25</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B36" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="C36" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="D36" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="E36" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="F36" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="G36" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="H36" s="11">
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B37" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="C37" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="D37" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="E37" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="F37" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="G37" s="16">
-        <v>7.25</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B37" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="C37" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="D37" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="E37" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="F37" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="G37" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="H37" s="11">
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B38" s="16">
+      <c r="B38" s="11">
         <v>7.3</v>
       </c>
-      <c r="C38" s="16">
+      <c r="C38" s="11">
         <v>7.4</v>
       </c>
-      <c r="D38" s="16">
+      <c r="D38" s="11">
         <v>7.7</v>
       </c>
-      <c r="E38" s="16">
+      <c r="E38" s="11">
         <v>7.85</v>
       </c>
-      <c r="F38" s="16">
+      <c r="F38" s="11">
         <v>7.95</v>
       </c>
-      <c r="G38" s="16">
+      <c r="G38" s="11">
         <v>8.1</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H38" s="11">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B39" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="C39" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="D39" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="E39" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="F39" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="G39" s="16">
-        <v>7.25</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B39" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="C39" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="D39" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="E39" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="F39" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="G39" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="H39" s="11">
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B40" s="16">
+      <c r="B40" s="11">
         <v>8.4</v>
       </c>
-      <c r="C40" s="16">
+      <c r="C40" s="11">
         <v>8.5</v>
       </c>
-      <c r="D40" s="16">
+      <c r="D40" s="11">
         <v>8.8000000000000007</v>
       </c>
-      <c r="E40" s="16">
+      <c r="E40" s="11">
         <v>8.9499999999999993</v>
       </c>
-      <c r="F40" s="16">
+      <c r="F40" s="11">
         <v>9.1</v>
       </c>
-      <c r="G40" s="16">
+      <c r="G40" s="11">
         <v>9.25</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H40" s="11">
+        <v>9.75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B41" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="C41" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="D41" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="E41" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="F41" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="G41" s="16">
-        <v>7.25</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B41" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="C41" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="D41" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="E41" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="F41" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="G41" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="H41" s="11">
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B42" s="16">
+      <c r="B42" s="11">
         <v>7.4</v>
       </c>
-      <c r="C42" s="16">
+      <c r="C42" s="11">
         <v>7.4</v>
       </c>
-      <c r="D42" s="16">
+      <c r="D42" s="11">
         <v>7.4</v>
       </c>
-      <c r="E42" s="16">
+      <c r="E42" s="11">
         <v>7.75</v>
       </c>
-      <c r="F42" s="16">
+      <c r="F42" s="11">
         <v>8</v>
       </c>
-      <c r="G42" s="16">
+      <c r="G42" s="11">
         <v>9</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H42" s="11">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B43" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="C43" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="D43" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="E43" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="F43" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="G43" s="16">
-        <v>7.25</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B43" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="C43" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="D43" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="E43" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="F43" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="G43" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="H43" s="11">
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B44" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="C44" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="D44" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="E44" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="F44" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="G44" s="16">
+      <c r="B44" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="C44" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="D44" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="E44" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="F44" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="G44" s="11">
         <v>8.5</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H44" s="11">
+        <v>8.5500000000000007</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B45" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="C45" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="D45" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="E45" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="F45" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="G45" s="16">
-        <v>7.25</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B45" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="C45" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="D45" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="E45" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="F45" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="G45" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="H45" s="11">
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B46" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="C46" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="D46" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="E46" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="F46" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="G46" s="16">
-        <v>7.25</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B46" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="C46" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="D46" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="E46" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="F46" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="G46" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="H46" s="11">
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B47" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="C47" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="D47" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="E47" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="F47" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="G47" s="16">
-        <v>7.25</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B47" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="C47" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="D47" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="E47" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="F47" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="G47" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="H47" s="11">
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B48" s="16">
+      <c r="B48" s="11">
         <v>8.06</v>
       </c>
-      <c r="C48" s="16">
+      <c r="C48" s="11">
         <v>8.15</v>
       </c>
-      <c r="D48" s="16">
+      <c r="D48" s="11">
         <v>8.4600000000000009</v>
       </c>
-      <c r="E48" s="16">
+      <c r="E48" s="11">
         <v>8.6</v>
       </c>
-      <c r="F48" s="16">
+      <c r="F48" s="11">
         <v>8.73</v>
       </c>
-      <c r="G48" s="16">
+      <c r="G48" s="11">
         <v>9.15</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H48" s="11">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B49" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="C49" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="D49" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="E49" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="F49" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="G49" s="16">
-        <v>7.25</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B49" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="C49" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="D49" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="E49" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="F49" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="G49" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="H49" s="11">
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B50" s="16">
+      <c r="B50" s="11">
         <v>8.5500000000000007</v>
       </c>
-      <c r="C50" s="16">
+      <c r="C50" s="11">
         <v>8.67</v>
       </c>
-      <c r="D50" s="16">
+      <c r="D50" s="11">
         <v>9.0399999999999991</v>
       </c>
-      <c r="E50" s="16">
+      <c r="E50" s="11">
         <v>9.19</v>
       </c>
-      <c r="F50" s="16">
+      <c r="F50" s="11">
         <v>9.32</v>
       </c>
-      <c r="G50" s="16">
+      <c r="G50" s="11">
         <v>9.4700000000000006</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H50" s="11">
+        <v>9.4700000000000006</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B51" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="C51" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="D51" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="E51" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="F51" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="G51" s="16">
+      <c r="B51" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="C51" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="D51" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="E51" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="F51" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="G51" s="11">
         <v>8</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H51" s="11">
+        <v>8.75</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A52" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B52" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="C52" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="D52" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="E52" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="F52" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="G52" s="16">
-        <v>7.25</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B52" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="C52" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="D52" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="E52" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="F52" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="G52" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="H52" s="11">
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B53" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="C53" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="D53" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="E53" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="F53" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="G53" s="16">
-        <v>7.25</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="15.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B53" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="C53" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="D53" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="E53" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="F53" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="G53" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="H53" s="11">
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="15.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A54" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B54" s="16">
+      <c r="B54" s="11">
         <v>8.25</v>
       </c>
-      <c r="C54" s="16">
+      <c r="C54" s="11">
         <v>8.25</v>
       </c>
-      <c r="D54" s="16">
+      <c r="D54" s="11">
         <v>8.25</v>
       </c>
-      <c r="E54" s="16">
+      <c r="E54" s="11">
         <v>8.25</v>
       </c>
-      <c r="F54" s="16">
+      <c r="F54" s="11">
         <v>9.5</v>
       </c>
-      <c r="G54" s="16">
+      <c r="G54" s="11">
         <v>10.5</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H54" s="11">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B55" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="C55" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="D55" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="E55" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="F55" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="G55" s="16">
+      <c r="B55" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="C55" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="D55" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="E55" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="F55" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="G55" s="11">
         <v>8.25</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H55" s="11">
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A56" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B56" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="C56" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="D56" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="E56" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="F56" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="G56" s="16">
-        <v>7.25</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="15.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B56" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="C56" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="D56" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="E56" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="F56" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="G56" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="H56" s="11">
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="15.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A57" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B57" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="C57" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="D57" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="E57" s="16">
-        <v>7.25</v>
-      </c>
-      <c r="F57" s="17">
-        <v>7.25</v>
-      </c>
-      <c r="G57" s="17">
+      <c r="B57" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="C57" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="D57" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="E57" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="F57" s="12">
+        <v>7.25</v>
+      </c>
+      <c r="G57" s="12">
+        <v>7.25</v>
+      </c>
+      <c r="H57" s="12">
         <v>7.25</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
@@ -2260,8 +2430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9D7972A-DAB7-4667-9950-F43F389AF8E5}">
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2270,25 +2440,25 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6">
+      <c r="B1" s="16">
         <v>2010</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6">
+      <c r="D1" s="16">
         <v>2012</v>
       </c>
-      <c r="E1" s="6">
+      <c r="E1" s="16">
         <v>2013</v>
       </c>
-      <c r="F1" s="6">
+      <c r="F1" s="16">
         <v>2014</v>
       </c>
-      <c r="G1" s="6">
+      <c r="G1" s="16">
         <v>2015</v>
       </c>
-      <c r="H1" s="6">
+      <c r="H1" s="16">
         <v>2016</v>
       </c>
     </row>
@@ -2296,13 +2466,13 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
     </row>
     <row r="3" spans="1:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">

</xml_diff>